<commit_message>
Scenarios on EMI packs and Slab Based Charges
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/4943-DisburseLoan-ChangeMeetingDate-MakeRepayment.xlsx
+++ b/Finflux Automation Excels/Client/4943-DisburseLoan-ChangeMeetingDate-MakeRepayment.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Center" sheetId="1" r:id="rId1"/>
     <sheet name="Group" sheetId="2" r:id="rId2"/>
     <sheet name="NewLoanInput" sheetId="3" r:id="rId3"/>
     <sheet name="Modify Transaction" sheetId="4" r:id="rId4"/>
+    <sheet name="Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="Repayment schedule" sheetId="6" r:id="rId6"/>
+    <sheet name="Transactions" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t>CenterVillageName</t>
   </si>
@@ -193,6 +196,90 @@
   </si>
   <si>
     <t>06 April 2015</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Waived</t>
+  </si>
+  <si>
+    <t>Written Off</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>Over Due</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Penalties</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Paid Date</t>
+  </si>
+  <si>
+    <t>Principal Due</t>
+  </si>
+  <si>
+    <t>Balance of Loan</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>In Advance</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>TransactionType</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Loan Balance</t>
+  </si>
+  <si>
+    <t>Head Office</t>
+  </si>
+  <si>
+    <t>Repayment (at time of disbursement)</t>
+  </si>
+  <si>
+    <t>Disbursement</t>
   </si>
 </sst>
 </file>
@@ -202,7 +289,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +307,22 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -254,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -272,6 +375,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +676,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +799,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +866,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,23 +1071,23 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -974,7 +1095,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">
@@ -982,10 +1103,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -993,4 +1114,868 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>5000</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12">
+        <v>5000</v>
+      </c>
+      <c r="F2" s="14">
+        <v>2049.92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>183.42</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>183.42</v>
+      </c>
+      <c r="F3" s="13">
+        <v>96.28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>150</v>
+      </c>
+      <c r="B4" s="13">
+        <v>150</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="15">
+        <v>42005</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12">
+        <v>5000</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13">
+        <v>150</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13">
+        <v>150</v>
+      </c>
+      <c r="L2" s="13">
+        <v>150</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>25</v>
+      </c>
+      <c r="C3" s="15">
+        <v>42030</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13">
+        <v>406.23</v>
+      </c>
+      <c r="G3" s="14">
+        <v>4593.7700000000004</v>
+      </c>
+      <c r="H3" s="13">
+        <v>23.01</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13">
+        <v>0</v>
+      </c>
+      <c r="O3" s="13">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>14</v>
+      </c>
+      <c r="C4" s="15">
+        <v>42044</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13">
+        <v>406.23</v>
+      </c>
+      <c r="G4" s="14">
+        <v>4187.54</v>
+      </c>
+      <c r="H4" s="13">
+        <v>23.01</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13">
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>14</v>
+      </c>
+      <c r="C5" s="15">
+        <v>42058</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13">
+        <v>406.23</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3781.31</v>
+      </c>
+      <c r="H5" s="13">
+        <v>23.01</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0</v>
+      </c>
+      <c r="K5" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13">
+        <v>14</v>
+      </c>
+      <c r="C6" s="15">
+        <v>42072</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13">
+        <v>406.23</v>
+      </c>
+      <c r="G6" s="14">
+        <v>3375.08</v>
+      </c>
+      <c r="H6" s="13">
+        <v>23.01</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13">
+        <v>14</v>
+      </c>
+      <c r="C7" s="15">
+        <v>42086</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
+        <v>406.23</v>
+      </c>
+      <c r="G7" s="14">
+        <v>2968.85</v>
+      </c>
+      <c r="H7" s="13">
+        <v>23.01</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <v>0</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13">
+        <v>21</v>
+      </c>
+      <c r="C8" s="15">
+        <v>42107</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13">
+        <v>402.74</v>
+      </c>
+      <c r="G8" s="14">
+        <v>2566.11</v>
+      </c>
+      <c r="H8" s="13">
+        <v>26.5</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0</v>
+      </c>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
+        <v>14</v>
+      </c>
+      <c r="C9" s="15">
+        <v>42121</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
+        <v>417.43</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2148.6799999999998</v>
+      </c>
+      <c r="H9" s="13">
+        <v>11.81</v>
+      </c>
+      <c r="I9" s="13">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="K9" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13">
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>14</v>
+      </c>
+      <c r="C10" s="15">
+        <v>42135</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13">
+        <v>419.35</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1729.33</v>
+      </c>
+      <c r="H10" s="13">
+        <v>9.89</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L10" s="13">
+        <v>0</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13">
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <v>0</v>
+      </c>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>14</v>
+      </c>
+      <c r="C11" s="15">
+        <v>42149</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13">
+        <v>421.28</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1308.05</v>
+      </c>
+      <c r="H11" s="13">
+        <v>7.96</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L11" s="13">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13">
+        <v>0</v>
+      </c>
+      <c r="O11" s="13">
+        <v>0</v>
+      </c>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13">
+        <v>14</v>
+      </c>
+      <c r="C12" s="15">
+        <v>42163</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13">
+        <v>423.22</v>
+      </c>
+      <c r="G12" s="13">
+        <v>884.83</v>
+      </c>
+      <c r="H12" s="13">
+        <v>6.02</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L12" s="13">
+        <v>0</v>
+      </c>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13">
+        <v>0</v>
+      </c>
+      <c r="O12" s="13">
+        <v>0</v>
+      </c>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15">
+        <v>42177</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13">
+        <v>425.17</v>
+      </c>
+      <c r="G13" s="13">
+        <v>459.66</v>
+      </c>
+      <c r="H13" s="13">
+        <v>4.07</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>429.24</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13">
+        <v>429.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>14</v>
+      </c>
+      <c r="C14" s="15">
+        <v>42191</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13">
+        <v>459.66</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>2.12</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <v>461.78</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13">
+        <v>0</v>
+      </c>
+      <c r="O14" s="13">
+        <v>0</v>
+      </c>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13">
+        <v>461.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>58</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="15">
+        <v>42005</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="13">
+        <v>150</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
+        <v>150</v>
+      </c>
+      <c r="I2" s="13">
+        <v>0</v>
+      </c>
+      <c r="J2" s="12">
+        <v>5000</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>57</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="15">
+        <v>42005</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="12">
+        <v>5000</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
+        <v>5000</v>
+      </c>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>